<commit_message>
Added fields from Simon's course to meta-data model.
</commit_message>
<xml_diff>
--- a/design/MetaDataModel.xlsx
+++ b/design/MetaDataModel.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="21975" windowHeight="12780"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19260" windowHeight="6255"/>
   </bookViews>
   <sheets>
     <sheet name="Session" sheetId="1" r:id="rId1"/>
     <sheet name="Person" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="File" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="166">
   <si>
     <t>Title</t>
   </si>
@@ -406,9 +406,6 @@
   </si>
   <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>English User Doc</t>
@@ -561,6 +558,139 @@
   </si>
   <si>
     <t>DON’T SHOW FOR NOW</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>WordCount</t>
+  </si>
+  <si>
+    <t>WordCount.IsEstimate</t>
+  </si>
+  <si>
+    <t>From Simons MD_Plan</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Will need to help with the estimate, by asking for a wpm  and multiplying times the recording length</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>Publishers</t>
+  </si>
+  <si>
+    <t>Recordist</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>DocumenterPeople</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Choice: Unknown, M, F</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>PlaceOfL1Learning</t>
+  </si>
+  <si>
+    <t>MothersLanguage</t>
+  </si>
+  <si>
+    <t>FathersLanguage</t>
+  </si>
+  <si>
+    <t>InformedConsentScan</t>
+  </si>
+  <si>
+    <t>Simons BOLD course</t>
+  </si>
+  <si>
+    <t>Simons, Mead.</t>
+  </si>
+  <si>
+    <t>Mead</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Bit Depth</t>
+  </si>
+  <si>
+    <t>Sampling Rate</t>
+  </si>
+  <si>
+    <t>Analog Gain</t>
+  </si>
+  <si>
+    <t>Digital Gain</t>
+  </si>
+  <si>
+    <t>RelativePath</t>
+  </si>
+  <si>
+    <t>The person who operated the recording device. In the case of a written task type, it identifies the person who operated the software to create the written transcription.</t>
+  </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>Person (0+)</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>TaskTypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial set: Original, Oral transcription, Oral translation, Oral discussion, Written transcription, Written translation, Written discussion
+</t>
+  </si>
+  <si>
+    <t>Devices</t>
+  </si>
+  <si>
+    <t>Channels</t>
+  </si>
+  <si>
+    <t>BitDepths</t>
+  </si>
+  <si>
+    <t>SamplingRates</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Initially: Open, Restricted</t>
+  </si>
+  <si>
+    <t>Notes that explain exactly what is in the file if there is more than one file for the same task type of the same item. The column should also be used to describe known problems in the recording.</t>
+  </si>
+  <si>
+    <t>Microphone</t>
   </si>
 </sst>
 </file>
@@ -643,7 +773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -651,13 +781,149 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:J44" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:J44"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Field"/>
+    <tableColumn id="2" name="Level"/>
+    <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Choices"/>
+    <tableColumn id="5" name="Required?"/>
+    <tableColumn id="6" name="Default"/>
+    <tableColumn id="7" name="Related Field in Mead's doc"/>
+    <tableColumn id="8" name="Notes"/>
+    <tableColumn id="9" name="English Field Name"/>
+    <tableColumn id="10" name="English User Doc"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J26" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:J26">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1"/>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Field"/>
+    <tableColumn id="2" name="EnglishFieldName"/>
+    <tableColumn id="3" name="Level"/>
+    <tableColumn id="4" name="Type"/>
+    <tableColumn id="5" name="Reuse in future"/>
+    <tableColumn id="6" name="Required?"/>
+    <tableColumn id="7" name="Default"/>
+    <tableColumn id="8" name="Source"/>
+    <tableColumn id="9" name="Notes"/>
+    <tableColumn id="10" name="English User Doc" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J15" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:J15"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Field"/>
+    <tableColumn id="2" name="Level"/>
+    <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Choices"/>
+    <tableColumn id="5" name="Required?"/>
+    <tableColumn id="6" name="Default"/>
+    <tableColumn id="7" name="Related Field in Mead's doc"/>
+    <tableColumn id="8" name="Notes"/>
+    <tableColumn id="9" name="English Field Name"/>
+    <tableColumn id="10" name="English User Doc"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -945,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -957,9 +1223,10 @@
     <col min="3" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1">
@@ -973,7 +1240,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>30</v>
@@ -988,35 +1255,35 @@
         <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1067,7 +1334,7 @@
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -1110,7 +1377,7 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" t="s">
         <v>36</v>
@@ -1119,7 +1386,7 @@
         <v>55</v>
       </c>
       <c r="I7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1142,7 +1409,7 @@
         <v>54</v>
       </c>
       <c r="I8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1165,7 +1432,7 @@
         <v>57</v>
       </c>
       <c r="I9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1193,7 +1460,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>38</v>
@@ -1213,7 +1480,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>40</v>
@@ -1258,7 +1525,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -1270,10 +1537,10 @@
         <v>36</v>
       </c>
       <c r="F14" t="s">
+        <v>120</v>
+      </c>
+      <c r="I14" t="s">
         <v>121</v>
-      </c>
-      <c r="I14" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1307,7 +1574,7 @@
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1707,13 +1974,13 @@
         <v>25</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C36" t="s">
         <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
       <c r="E36" t="s">
         <v>36</v>
@@ -1727,13 +1994,13 @@
         <v>26</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E37" t="s">
         <v>36</v>
@@ -1747,7 +2014,7 @@
         <v>27</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C38" t="s">
         <v>39</v>
@@ -1800,21 +2067,104 @@
       </c>
       <c r="I40" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" t="s">
+        <v>123</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>128</v>
+      </c>
+      <c r="D42" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" t="s">
+        <v>132</v>
+      </c>
+      <c r="E43" t="s">
+        <v>36</v>
+      </c>
+      <c r="G43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44" t="s">
+        <v>162</v>
+      </c>
+      <c r="H44" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1823,7 +2173,8 @@
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
     <col min="10" max="10" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1832,7 +2183,7 @@
         <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>60</v>
@@ -1850,46 +2201,46 @@
         <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="1" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1904,21 +2255,24 @@
         <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>141</v>
+      </c>
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" hidden="1">
       <c r="A4" t="s">
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
@@ -1930,10 +2284,10 @@
         <v>31</v>
       </c>
       <c r="H4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" hidden="1">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1953,15 +2307,15 @@
         <v>36</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" hidden="1">
       <c r="A6" t="s">
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C6">
         <v>9</v>
@@ -1984,10 +2338,10 @@
         <v>64</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E7" t="s">
         <v>36</v>
@@ -1996,7 +2350,7 @@
         <v>36</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2004,7 +2358,7 @@
         <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2019,15 +2373,15 @@
         <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" hidden="1">
       <c r="A9" t="s">
         <v>66</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -2044,10 +2398,10 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2056,15 +2410,15 @@
         <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2073,7 +2427,10 @@
         <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="H11" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2081,7 +2438,7 @@
         <v>67</v>
       </c>
       <c r="B12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2090,18 +2447,21 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" t="s">
         <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75">
       <c r="A13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -2110,26 +2470,28 @@
         <v>34</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" t="s">
+        <v>142</v>
+      </c>
       <c r="I13" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -2138,15 +2500,17 @@
         <v>34</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="H14" t="s">
+        <v>142</v>
+      </c>
       <c r="I14" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J14" s="4"/>
     </row>
@@ -2164,18 +2528,20 @@
         <v>34</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="H15" t="s">
+        <v>142</v>
+      </c>
       <c r="I15" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75">
@@ -2192,18 +2558,20 @@
         <v>34</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="H16" t="s">
+        <v>142</v>
+      </c>
       <c r="I16" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75">
@@ -2211,7 +2579,7 @@
         <v>70</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2220,13 +2588,16 @@
         <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F17" t="s">
         <v>36</v>
       </c>
+      <c r="H17" t="s">
+        <v>142</v>
+      </c>
       <c r="J17" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75">
@@ -2234,7 +2605,7 @@
         <v>71</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -2243,13 +2614,16 @@
         <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
         <v>36</v>
       </c>
+      <c r="H18" t="s">
+        <v>142</v>
+      </c>
       <c r="J18" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75">
@@ -2257,7 +2631,7 @@
         <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -2271,8 +2645,11 @@
       <c r="F19" t="s">
         <v>36</v>
       </c>
+      <c r="H19" t="s">
+        <v>142</v>
+      </c>
       <c r="J19" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -2280,7 +2657,7 @@
         <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -2293,6 +2670,9 @@
       </c>
       <c r="F20" t="s">
         <v>36</v>
+      </c>
+      <c r="H20" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -2314,22 +2694,326 @@
       <c r="F21" t="s">
         <v>36</v>
       </c>
+      <c r="H21" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75">
+      <c r="A22" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.75">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.75">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="I26" s="7"/>
+      <c r="J26" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="1" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>158</v>
+      </c>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
metadata model spreadsheet work
</commit_message>
<xml_diff>
--- a/design/MetaDataModel.xlsx
+++ b/design/MetaDataModel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19260" windowHeight="6255"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="16725" windowHeight="9675" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Session" sheetId="1" r:id="rId1"/>
@@ -808,6 +808,23 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -840,30 +857,13 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:J44" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:J44" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:J44"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Field"/>
@@ -901,14 +901,14 @@
     <tableColumn id="7" name="Default"/>
     <tableColumn id="8" name="Source"/>
     <tableColumn id="9" name="Notes"/>
-    <tableColumn id="10" name="English User Doc" dataDxfId="3"/>
+    <tableColumn id="10" name="English User Doc" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J15" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J15" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:J15"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Field"/>
@@ -1213,7 +1213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -2163,7 +2163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>